<commit_message>
Updated readme, used a serialized format to create characters info, added metronome.
</commit_message>
<xml_diff>
--- a/Logic/Basic Logic.xlsx
+++ b/Logic/Basic Logic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dysmse5-my.sharepoint.com/personal/donald_intergriture_com/Documents/Documents/Intergriture/The Quest - ITG/Logic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="11_F25DC773A252ABDACC10484479DF43E85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCAC5D0F-6E00-4DE1-A2A6-B65660AD1078}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="11_F25DC773A252ABDACC10484479DF43E85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BF39AD0-6D40-4872-AB7C-288AA7475A38}"/>
   <bookViews>
-    <workbookView xWindow="12480" yWindow="0" windowWidth="13210" windowHeight="13770" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>王室公主</t>
   </si>
   <si>
-    <t>Chasity</t>
-  </si>
-  <si>
     <t>白浊法师</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>1 edging(until untied); cum: HP-3</t>
+  </si>
+  <si>
+    <t>Chastity</t>
   </si>
 </sst>
 </file>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,7 +686,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -704,7 +704,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -715,22 +715,22 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -738,28 +738,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -767,22 +767,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>27</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -790,28 +790,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -819,28 +819,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>39</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>40</v>
       </c>
-      <c r="I6" t="s">
-        <v>41</v>
-      </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -848,19 +848,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -868,25 +868,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>50</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
         <v>51</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -894,31 +894,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>56</v>
       </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" t="s">
-        <v>57</v>
-      </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" t="s">
         <v>59</v>
-      </c>
-      <c r="J9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -926,22 +926,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
         <v>61</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>62</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" t="s">
         <v>63</v>
       </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>64</v>
-      </c>
-      <c r="J10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -949,22 +949,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
         <v>66</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
         <v>67</v>
       </c>
-      <c r="G11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>68</v>
-      </c>
-      <c r="J11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -972,28 +972,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>71</v>
       </c>
-      <c r="E12" t="s">
-        <v>72</v>
-      </c>
       <c r="F12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
         <v>74</v>
       </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>75</v>
-      </c>
-      <c r="J12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1001,22 +1001,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" t="s">
         <v>77</v>
       </c>
-      <c r="D13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>78</v>
-      </c>
-      <c r="J13" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B83D7C-B639-49B1-BE50-B5C6AD36DC9C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="C4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1061,13 +1061,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
         <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1075,13 +1075,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
         <v>88</v>
-      </c>
-      <c r="E3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1089,10 +1089,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1100,10 +1100,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
         <v>91</v>
-      </c>
-      <c r="E5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1111,10 +1111,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
         <v>94</v>
-      </c>
-      <c r="E6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1122,10 +1122,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
         <v>96</v>
-      </c>
-      <c r="E7" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>